<commit_message>
dataset rename to english adjust code to this, update dnn results with validation set
</commit_message>
<xml_diff>
--- a/final_work/dataset/dataset_with_groups_and_time.xlsx
+++ b/final_work/dataset/dataset_with_groups_and_time.xlsx
@@ -446,82 +446,82 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Csoport</t>
+          <t>Group</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>1. röpZH</t>
+          <t>First_Weekly_Exam</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>2. röpZH</t>
+          <t>Second_Weekly_Exam</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>3. röpZH</t>
+          <t>Third_Weekly_Exam</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>4. röpZH</t>
+          <t>Fourth_Weekly_Exam</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>5. röpZH</t>
+          <t>Fifth_Weekly_Exam</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>6. röpZH</t>
+          <t>Sixth_Weekly_Exam</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>7. röpZH</t>
+          <t>Seventh_Weekly_Exam</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>8. röpZH</t>
+          <t>Eighth_Weekly_Exam</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>9. röpZH</t>
+          <t>Ninth_Weekly_Exam</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>10. röpZH</t>
+          <t>Tenth_Weekly_Exam</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Beadandó</t>
+          <t>Assignment</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>ZH</t>
+          <t>Final_Exam</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Nap</t>
+          <t>Day</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Óra</t>
+          <t>Start_Hour</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>+1 (javító) röpZH</t>
+          <t>Bonus_Weekly_Exam_Retake</t>
         </is>
       </c>
     </row>

</xml_diff>